<commit_message>
Changement dans le dictionaire de donnees
</commit_message>
<xml_diff>
--- a/Doc/Dictionaire.xlsx
+++ b/Doc/Dictionaire.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lille\universite_de_Lille\Archi_et_donnees_du_Web_Mr_Marcq\TP_Note\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E67596A-63EB-4625-8952-AD1A39EF24BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C2B4643-8232-4351-8B68-EF67F5D39FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>TINYINT</t>
   </si>
   <si>
-    <t>Identifiant du rôle</t>
-  </si>
-  <si>
     <t>libelle</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>Nom de l’objet (arme, accessoire)</t>
+  </si>
+  <si>
+    <t>Identifiant du role</t>
   </si>
 </sst>
 </file>
@@ -532,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="79" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,111 +621,111 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="22" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:5" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -737,67 +737,67 @@
         <v>6</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>